<commit_message>
Percentage Formatting for Tableau
</commit_message>
<xml_diff>
--- a/Resources/All_stats.xlsx
+++ b/Resources/All_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian Keffer\GW Bootcamp\Project-4\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pfeff\OneDrive\Documents\GitHubRepositories\Project-4\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA961CC0-274A-43C4-849B-340502201A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A212B0A-0BD6-4D22-8F15-938DA094A1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6070C290-6BE5-4A56-A6A7-E34EA935CACA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{6070C290-6BE5-4A56-A6A7-E34EA935CACA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,10 +132,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +143,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -168,8 +172,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -179,15 +184,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -203,9 +209,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -243,7 +249,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -349,7 +355,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -491,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -502,3880 +508,3880 @@
   <dimension ref="A1:F217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I184" sqref="I184"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>541</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>5.5E-2</v>
       </c>
       <c r="D2" s="2">
         <v>93125</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F2" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>7909</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>0.13</v>
       </c>
       <c r="D3" s="2">
         <v>361671</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F3" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>7998</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="D4" s="2">
         <v>158067</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="F4" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2">
         <v>9890</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="D5" s="2">
         <v>249652</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F5" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2">
         <v>1451</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>0.15</v>
       </c>
       <c r="D6" s="2">
         <v>311314</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F6" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>393</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>-2.8000000000000001E-2</v>
       </c>
       <c r="D7" s="2">
         <v>154011</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="F7" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>2148</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>0.161</v>
       </c>
       <c r="D8" s="2">
         <v>298873</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F8" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>1184</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>0.13100000000000001</v>
       </c>
       <c r="D9" s="2">
         <v>218225</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="4">
         <v>-7.0000000000000001E-3</v>
       </c>
       <c r="F9" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2">
         <v>2348</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>0.13300000000000001</v>
       </c>
       <c r="D10" s="2">
         <v>269921</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="F10" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2">
         <v>402</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>0.122</v>
       </c>
       <c r="D11" s="2">
         <v>167923</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>-2.1999999999999999E-2</v>
       </c>
       <c r="F11" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2">
         <v>3726</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>0.11799999999999999</v>
       </c>
       <c r="D12" s="2">
         <v>295621</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F12" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2">
         <v>399</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="4">
         <v>0.17499999999999999</v>
       </c>
       <c r="D13" s="2">
         <v>285670</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="F13" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2">
         <v>3397</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>0.11</v>
       </c>
       <c r="D14" s="2">
         <v>260212</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4">
         <v>1.6E-2</v>
       </c>
       <c r="F14" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2">
         <v>4128</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <v>0.10299999999999999</v>
       </c>
       <c r="D15" s="2">
         <v>432329</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F15" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="2">
         <v>275</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <v>0.185</v>
       </c>
       <c r="D16" s="2">
         <v>232027</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="4">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="F16" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="2">
         <v>12176</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="4">
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="D17" s="2">
         <v>501093</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="4">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F17" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="2">
         <v>9350</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="4">
         <v>0.104</v>
       </c>
       <c r="D18" s="2">
         <v>248828</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="4">
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F18" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="2">
         <v>833</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="4">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="D19" s="2">
         <v>331776</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="4">
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="F19" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="2">
         <v>216</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="4">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="D20" s="2">
         <v>90290</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="4">
         <v>0.28499999999999998</v>
       </c>
       <c r="F20" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="2">
         <v>1368</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="4">
         <v>0.11600000000000001</v>
       </c>
       <c r="D21" s="2">
         <v>262345</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="4">
         <v>6.3E-2</v>
       </c>
       <c r="F21" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2">
         <v>617</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="4">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="D22" s="2">
         <v>399773</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="4">
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F22" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="2">
         <v>1634</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="4">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="D23" s="2">
         <v>178559</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="4">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F23" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="2">
         <v>1079</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="4">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="D24" s="2">
         <v>154160</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="4">
         <v>-0.02</v>
       </c>
       <c r="F24" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="2">
         <v>2019</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D25" s="2">
         <v>254423</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="4">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F25" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>3</v>
       </c>
       <c r="B26" s="2">
         <v>571</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="4">
         <v>0.13500000000000001</v>
       </c>
       <c r="D26" s="2">
         <v>96286</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="4">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F26" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>4</v>
       </c>
       <c r="B27" s="2">
         <v>8938</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="4">
         <v>1.4E-2</v>
       </c>
       <c r="D27" s="2">
         <v>369780</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="4">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F27" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="2">
         <v>8537</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="4">
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="D28" s="2">
         <v>172429</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="4">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F28" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="2">
         <v>10727</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="4">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="D29" s="2">
         <v>262855</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="4">
         <v>0.05</v>
       </c>
       <c r="F29" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="2">
         <v>1669</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="4">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="D30" s="2">
         <v>313830</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="4">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="F30" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="2">
         <v>382</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="4">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="D31" s="2">
         <v>167711</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="4">
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="F31" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>9</v>
       </c>
       <c r="B32" s="2">
         <v>2493</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="4">
         <v>-4.4999999999999998E-2</v>
       </c>
       <c r="D32" s="2">
         <v>313141</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="4">
         <v>0.05</v>
       </c>
       <c r="F32" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>10</v>
       </c>
       <c r="B33" s="2">
         <v>1339</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="4">
         <v>5.5E-2</v>
       </c>
       <c r="D33" s="2">
         <v>216604</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="4">
         <v>0.05</v>
       </c>
       <c r="F33" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="2">
         <v>2660</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="4">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="D34" s="2">
         <v>281123</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="4">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="F34" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="2">
         <v>451</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="4">
         <v>-7.0999999999999994E-2</v>
       </c>
       <c r="D35" s="2">
         <v>164247</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="4">
         <v>0.105</v>
       </c>
       <c r="F35" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>13</v>
       </c>
       <c r="B36" s="2">
         <v>4164</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="4">
         <v>0.08</v>
       </c>
       <c r="D36" s="2">
         <v>303453</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="4">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="F36" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>14</v>
       </c>
       <c r="B37" s="2">
         <v>469</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="4">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="D37" s="2">
         <v>299765</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="4">
         <v>0.23</v>
       </c>
       <c r="F37" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>15</v>
       </c>
       <c r="B38" s="2">
         <v>3772</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="4">
         <v>1.6E-2</v>
       </c>
       <c r="D38" s="2">
         <v>264334</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="4">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F38" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="2">
         <v>4554</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D39" s="2">
         <v>434384</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="4">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F39" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>17</v>
       </c>
       <c r="B40" s="2">
         <v>326</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="4">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D40" s="2">
         <v>251150</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="4">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="F40" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="2">
         <v>12865</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="4">
         <v>-5.0000000000000001E-3</v>
       </c>
       <c r="D41" s="2">
         <v>505003</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="4">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="F41" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="2">
         <v>10322</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="4">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="D42" s="2">
         <v>266947</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="4">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="F42" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>20</v>
       </c>
       <c r="B43" s="2">
         <v>860</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="4">
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="D43" s="2">
         <v>355763</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="4">
         <v>2.4E-2</v>
       </c>
       <c r="F43" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>21</v>
       </c>
       <c r="B44" s="2">
         <v>233</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="4">
         <v>-6.4000000000000001E-2</v>
       </c>
       <c r="D44" s="2">
         <v>116013</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="F44" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="2">
         <v>1527</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="4">
         <v>0.09</v>
       </c>
       <c r="D45" s="2">
         <v>278823</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="4">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F45" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>23</v>
       </c>
       <c r="B46" s="2">
         <v>630</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="4">
         <v>0.11700000000000001</v>
       </c>
       <c r="D46" s="2">
         <v>406660</v>
       </c>
-      <c r="E46" s="3">
+      <c r="E46" s="4">
         <v>0.13100000000000001</v>
       </c>
       <c r="F46" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="2">
         <v>1784</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="4">
         <v>0</v>
       </c>
       <c r="D47" s="2">
         <v>188092</v>
       </c>
-      <c r="E47" s="3">
+      <c r="E47" s="4">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="F47" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>25</v>
       </c>
       <c r="B48" s="2">
         <v>1156</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="4">
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="D48" s="2">
         <v>151027</v>
       </c>
-      <c r="E48" s="3">
+      <c r="E48" s="4">
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="F48" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>26</v>
       </c>
       <c r="B49" s="2">
         <v>2160</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="4">
         <v>0.122</v>
       </c>
       <c r="D49" s="2">
         <v>261507</v>
       </c>
-      <c r="E49" s="3">
+      <c r="E49" s="4">
         <v>0.05</v>
       </c>
       <c r="F49" s="2">
         <v>2016</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>3</v>
       </c>
       <c r="B50" s="2">
         <v>648</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="4">
         <v>-0.04</v>
       </c>
       <c r="D50" s="2">
         <v>97097</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E50" s="4">
         <v>0.122</v>
       </c>
       <c r="F50" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>4</v>
       </c>
       <c r="B51" s="2">
         <v>9060</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D51" s="2">
         <v>386316</v>
       </c>
-      <c r="E51" s="3">
+      <c r="E51" s="4">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="F51" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>5</v>
       </c>
       <c r="B52" s="2">
         <v>9379</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="4">
         <v>-3.4000000000000002E-2</v>
       </c>
       <c r="D52" s="2">
         <v>180785</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E52" s="4">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="F52" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>6</v>
       </c>
       <c r="B53" s="2">
         <v>10890</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="4">
         <v>-0.02</v>
       </c>
       <c r="D53" s="2">
         <v>275893</v>
       </c>
-      <c r="E53" s="3">
+      <c r="E53" s="4">
         <v>2.7E-2</v>
       </c>
       <c r="F53" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>7</v>
       </c>
       <c r="B54" s="2">
         <v>1737</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="4">
         <v>-3.5999999999999997E-2</v>
       </c>
       <c r="D54" s="2">
         <v>338544</v>
       </c>
-      <c r="E54" s="3">
+      <c r="E54" s="4">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="F54" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="2">
         <v>390</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="4">
         <v>-7.1999999999999995E-2</v>
       </c>
       <c r="D55" s="2">
         <v>179998</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E55" s="4">
         <v>0.06</v>
       </c>
       <c r="F55" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>9</v>
       </c>
       <c r="B56" s="2">
         <v>2382</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="4">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="D56" s="2">
         <v>328715</v>
       </c>
-      <c r="E56" s="3">
+      <c r="E56" s="4">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F56" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>10</v>
       </c>
       <c r="B57" s="2">
         <v>1412</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="4">
         <v>-6.6000000000000003E-2</v>
       </c>
       <c r="D57" s="2">
         <v>227371</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="4">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F57" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>11</v>
       </c>
       <c r="B58" s="2">
         <v>2832</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="4">
         <v>-2.5999999999999999E-2</v>
       </c>
       <c r="D58" s="2">
         <v>295701</v>
       </c>
-      <c r="E58" s="3">
+      <c r="E58" s="4">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="F58" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>12</v>
       </c>
       <c r="B59" s="2">
         <v>419</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="4">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="D59" s="2">
         <v>181483</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="4">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="F59" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>13</v>
       </c>
       <c r="B60" s="2">
         <v>4497</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="4">
         <v>-1.2E-2</v>
       </c>
       <c r="D60" s="2">
         <v>322778</v>
       </c>
-      <c r="E60" s="3">
+      <c r="E60" s="4">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="F60" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>14</v>
       </c>
       <c r="B61" s="2">
         <v>496</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="4">
         <v>-3.4000000000000002E-2</v>
       </c>
       <c r="D61" s="2">
         <v>368860</v>
       </c>
-      <c r="E61" s="3">
+      <c r="E61" s="4">
         <v>-8.4000000000000005E-2</v>
       </c>
       <c r="F61" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>15</v>
       </c>
       <c r="B62" s="2">
         <v>3831</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="4">
         <v>2.3E-2</v>
       </c>
       <c r="D62" s="2">
         <v>273315</v>
       </c>
-      <c r="E62" s="3">
+      <c r="E62" s="4">
         <v>0.03</v>
       </c>
       <c r="F62" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>16</v>
       </c>
       <c r="B63" s="2">
         <v>4583</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="4">
         <v>-4.8000000000000001E-2</v>
       </c>
       <c r="D63" s="2">
         <v>445808</v>
       </c>
-      <c r="E63" s="3">
+      <c r="E63" s="4">
         <v>2.3E-2</v>
       </c>
       <c r="F63" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>17</v>
       </c>
       <c r="B64" s="2">
         <v>334</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="4">
         <v>-0.03</v>
       </c>
       <c r="D64" s="2">
         <v>260472</v>
       </c>
-      <c r="E64" s="3">
+      <c r="E64" s="4">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="F64" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>18</v>
       </c>
       <c r="B65" s="2">
         <v>12802</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="4">
         <v>-2.5999999999999999E-2</v>
       </c>
       <c r="D65" s="2">
         <v>522213</v>
       </c>
-      <c r="E65" s="3">
+      <c r="E65" s="4">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="F65" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="2">
         <v>11028</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66" s="4">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="D66" s="2">
         <v>289587</v>
       </c>
-      <c r="E66" s="3">
+      <c r="E66" s="4">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="F66" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>20</v>
       </c>
       <c r="B67" s="2">
         <v>931</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="4">
         <v>-6.2E-2</v>
       </c>
       <c r="D67" s="2">
         <v>364340</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E67" s="4">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F67" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>21</v>
       </c>
       <c r="B68" s="2">
         <v>218</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="4">
         <v>0.06</v>
       </c>
       <c r="D68" s="2">
         <v>122903</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E68" s="4">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="F68" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>22</v>
       </c>
       <c r="B69" s="2">
         <v>1664</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="4">
         <v>-1.6E-2</v>
       </c>
       <c r="D69" s="2">
         <v>288713</v>
       </c>
-      <c r="E69" s="3">
+      <c r="E69" s="4">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="F69" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="2">
         <v>704</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="4">
         <v>-0.06</v>
       </c>
       <c r="D70" s="2">
         <v>460055</v>
       </c>
-      <c r="E70" s="3">
+      <c r="E70" s="4">
         <v>-1.9E-2</v>
       </c>
       <c r="F70" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>24</v>
       </c>
       <c r="B71" s="2">
         <v>1784</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="D71" s="2">
         <v>199209</v>
       </c>
-      <c r="E71" s="3">
+      <c r="E71" s="4">
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="F71" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>25</v>
       </c>
       <c r="B72" s="2">
         <v>1255</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="4">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="D72" s="2">
         <v>161207</v>
       </c>
-      <c r="E72" s="3">
+      <c r="E72" s="4">
         <v>2.9000000000000001E-2</v>
       </c>
       <c r="F72" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>26</v>
       </c>
       <c r="B73" s="2">
         <v>2424</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="4">
         <v>-4.1000000000000002E-2</v>
       </c>
       <c r="D73" s="2">
         <v>274495</v>
       </c>
-      <c r="E73" s="3">
+      <c r="E73" s="4">
         <v>0.04</v>
       </c>
       <c r="F73" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>3</v>
       </c>
       <c r="B74" s="1">
         <v>622</v>
       </c>
-      <c r="C74" s="4">
+      <c r="C74" s="3">
         <v>0.11700000000000001</v>
       </c>
       <c r="D74" s="1">
         <v>108916</v>
       </c>
-      <c r="E74" s="4">
+      <c r="E74" s="3">
         <v>2.4E-2</v>
       </c>
       <c r="F74" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>4</v>
       </c>
       <c r="B75" s="1">
         <v>9112</v>
       </c>
-      <c r="C75" s="4">
+      <c r="C75" s="3">
         <v>0.10100000000000001</v>
       </c>
       <c r="D75" s="1">
         <v>403349</v>
       </c>
-      <c r="E75" s="4">
+      <c r="E75" s="3">
         <v>0.02</v>
       </c>
       <c r="F75" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>5</v>
       </c>
       <c r="B76" s="1">
         <v>9057</v>
       </c>
-      <c r="C76" s="4">
+      <c r="C76" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D76" s="1">
         <v>182088</v>
       </c>
-      <c r="E76" s="4">
+      <c r="E76" s="3">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F76" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>6</v>
       </c>
       <c r="B77" s="1">
         <v>10669</v>
       </c>
-      <c r="C77" s="4">
+      <c r="C77" s="3">
         <v>2.7E-2</v>
       </c>
       <c r="D77" s="1">
         <v>283423</v>
       </c>
-      <c r="E77" s="4">
+      <c r="E77" s="3">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="F77" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>7</v>
       </c>
       <c r="B78" s="1">
         <v>1675</v>
       </c>
-      <c r="C78" s="4">
+      <c r="C78" s="3">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="D78" s="1">
         <v>350956</v>
       </c>
-      <c r="E78" s="4">
+      <c r="E78" s="3">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="F78" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="1">
         <v>362</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C79" s="3">
         <v>0.21299999999999999</v>
       </c>
       <c r="D79" s="1">
         <v>190836</v>
       </c>
-      <c r="E79" s="4">
+      <c r="E79" s="3">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F79" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>9</v>
       </c>
       <c r="B80" s="1">
         <v>2390</v>
       </c>
-      <c r="C80" s="4">
+      <c r="C80" s="3">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D80" s="1">
         <v>338010</v>
       </c>
-      <c r="E80" s="4">
+      <c r="E80" s="3">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="F80" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>10</v>
       </c>
       <c r="B81" s="1">
         <v>1319</v>
       </c>
-      <c r="C81" s="4">
+      <c r="C81" s="3">
         <v>0.121</v>
       </c>
       <c r="D81" s="1">
         <v>235309</v>
       </c>
-      <c r="E81" s="4">
+      <c r="E81" s="3">
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="F81" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>11</v>
       </c>
       <c r="B82" s="1">
         <v>2757</v>
       </c>
-      <c r="C82" s="4">
+      <c r="C82" s="3">
         <v>0.125</v>
       </c>
       <c r="D82" s="1">
         <v>311739</v>
       </c>
-      <c r="E82" s="4">
+      <c r="E82" s="3">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="F82" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>12</v>
       </c>
       <c r="B83" s="1">
         <v>434</v>
       </c>
-      <c r="C83" s="4">
+      <c r="C83" s="3">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="D83" s="1">
         <v>194048</v>
       </c>
-      <c r="E83" s="4">
+      <c r="E83" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F83" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>13</v>
       </c>
       <c r="B84" s="1">
         <v>4445</v>
       </c>
-      <c r="C84" s="4">
+      <c r="C84" s="3">
         <v>1.2E-2</v>
       </c>
       <c r="D84" s="1">
         <v>341426</v>
       </c>
-      <c r="E84" s="4">
+      <c r="E84" s="3">
         <v>2.4E-2</v>
       </c>
       <c r="F84" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>14</v>
       </c>
       <c r="B85" s="1">
         <v>479</v>
       </c>
-      <c r="C85" s="4">
+      <c r="C85" s="3">
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="D85" s="1">
         <v>337954</v>
       </c>
-      <c r="E85" s="4">
+      <c r="E85" s="3">
         <v>0.03</v>
       </c>
       <c r="F85" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>15</v>
       </c>
       <c r="B86" s="1">
         <v>3919</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86" s="3">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="D86" s="1">
         <v>281578</v>
       </c>
-      <c r="E86" s="4">
+      <c r="E86" s="3">
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="F86" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>16</v>
       </c>
       <c r="B87" s="1">
         <v>4362</v>
       </c>
-      <c r="C87" s="4">
+      <c r="C87" s="3">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="D87" s="1">
         <v>456190</v>
       </c>
-      <c r="E87" s="4">
+      <c r="E87" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="F87" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>17</v>
       </c>
       <c r="B88" s="1">
         <v>324</v>
       </c>
-      <c r="C88" s="4">
+      <c r="C88" s="3">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="D88" s="1">
         <v>278301</v>
       </c>
-      <c r="E88" s="4">
+      <c r="E88" s="3">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F88" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>18</v>
       </c>
       <c r="B89" s="1">
         <v>12471</v>
       </c>
-      <c r="C89" s="4">
+      <c r="C89" s="3">
         <v>2.7E-2</v>
       </c>
       <c r="D89" s="1">
         <v>540288</v>
       </c>
-      <c r="E89" s="4">
+      <c r="E89" s="3">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F89" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>19</v>
       </c>
       <c r="B90" s="1">
         <v>11175</v>
       </c>
-      <c r="C90" s="4">
+      <c r="C90" s="3">
         <v>3.9E-2</v>
       </c>
       <c r="D90" s="1">
         <v>302049</v>
       </c>
-      <c r="E90" s="4">
+      <c r="E90" s="3">
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="F90" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>20</v>
       </c>
       <c r="B91" s="1">
         <v>873</v>
       </c>
-      <c r="C91" s="4">
+      <c r="C91" s="3">
         <v>2E-3</v>
       </c>
       <c r="D91" s="1">
         <v>374633</v>
       </c>
-      <c r="E91" s="4">
+      <c r="E91" s="3">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F91" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>21</v>
       </c>
       <c r="B92" s="1">
         <v>231</v>
       </c>
-      <c r="C92" s="4">
+      <c r="C92" s="3">
         <v>0.16500000000000001</v>
       </c>
       <c r="D92" s="1">
         <v>128103</v>
       </c>
-      <c r="E92" s="4">
+      <c r="E92" s="3">
         <v>0.13600000000000001</v>
       </c>
       <c r="F92" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>22</v>
       </c>
       <c r="B93" s="1">
         <v>1638</v>
       </c>
-      <c r="C93" s="4">
+      <c r="C93" s="3">
         <v>0.129</v>
       </c>
       <c r="D93" s="1">
         <v>294659</v>
       </c>
-      <c r="E93" s="4">
+      <c r="E93" s="3">
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="F93" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>23</v>
       </c>
       <c r="B94" s="1">
         <v>662</v>
       </c>
-      <c r="C94" s="4">
+      <c r="C94" s="3">
         <v>-3.3000000000000002E-2</v>
       </c>
       <c r="D94" s="1">
         <v>451318</v>
       </c>
-      <c r="E94" s="4">
+      <c r="E94" s="3">
         <v>0.14799999999999999</v>
       </c>
       <c r="F94" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>24</v>
       </c>
       <c r="B95" s="1">
         <v>1794</v>
       </c>
-      <c r="C95" s="4">
+      <c r="C95" s="3">
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="D95" s="1">
         <v>214634</v>
       </c>
-      <c r="E95" s="4">
+      <c r="E95" s="3">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="F95" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>25</v>
       </c>
       <c r="B96" s="1">
         <v>1269</v>
       </c>
-      <c r="C96" s="4">
+      <c r="C96" s="3">
         <v>-4.3999999999999997E-2</v>
       </c>
       <c r="D96" s="1">
         <v>165808</v>
       </c>
-      <c r="E96" s="4">
+      <c r="E96" s="3">
         <v>0.11899999999999999</v>
       </c>
       <c r="F96" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>26</v>
       </c>
       <c r="B97" s="1">
         <v>2325</v>
       </c>
-      <c r="C97" s="4">
+      <c r="C97" s="3">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="D97" s="1">
         <v>285397</v>
       </c>
-      <c r="E97" s="4">
+      <c r="E97" s="3">
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="F97" s="1">
         <v>2018</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>3</v>
       </c>
       <c r="B98" s="1">
         <v>695</v>
       </c>
-      <c r="C98" s="4">
+      <c r="C98" s="3">
         <v>0.106</v>
       </c>
       <c r="D98" s="1">
         <v>111568</v>
       </c>
-      <c r="E98" s="4">
+      <c r="E98" s="3">
         <v>0.121</v>
       </c>
       <c r="F98" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>4</v>
       </c>
       <c r="B99" s="1">
         <v>10033</v>
       </c>
-      <c r="C99" s="4">
+      <c r="C99" s="3">
         <v>0.121</v>
       </c>
       <c r="D99" s="1">
         <v>411407</v>
       </c>
-      <c r="E99" s="4">
+      <c r="E99" s="3">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="F99" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>5</v>
       </c>
       <c r="B100" s="1">
         <v>9102</v>
       </c>
-      <c r="C100" s="4">
+      <c r="C100" s="3">
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="D100" s="1">
         <v>186893</v>
       </c>
-      <c r="E100" s="4">
+      <c r="E100" s="3">
         <v>0.106</v>
       </c>
       <c r="F100" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>6</v>
       </c>
       <c r="B101" s="1">
         <v>10953</v>
       </c>
-      <c r="C101" s="4">
+      <c r="C101" s="3">
         <v>6.3E-2</v>
       </c>
       <c r="D101" s="1">
         <v>294006</v>
       </c>
-      <c r="E101" s="4">
+      <c r="E101" s="3">
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="F101" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>7</v>
       </c>
       <c r="B102" s="1">
         <v>1738</v>
       </c>
-      <c r="C102" s="4">
+      <c r="C102" s="3">
         <v>0.159</v>
       </c>
       <c r="D102" s="1">
         <v>366356</v>
       </c>
-      <c r="E102" s="4">
+      <c r="E102" s="3">
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="F102" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>8</v>
       </c>
       <c r="B103" s="1">
         <v>439</v>
       </c>
-      <c r="C103" s="4">
+      <c r="C103" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="D103" s="1">
         <v>199362</v>
       </c>
-      <c r="E103" s="4">
+      <c r="E103" s="3">
         <v>0.13600000000000001</v>
       </c>
       <c r="F103" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>9</v>
       </c>
       <c r="B104" s="1">
         <v>2473</v>
       </c>
-      <c r="C104" s="4">
+      <c r="C104" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="D104" s="1">
         <v>348752</v>
       </c>
-      <c r="E104" s="4">
+      <c r="E104" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F104" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>10</v>
       </c>
       <c r="B105" s="1">
         <v>1478</v>
       </c>
-      <c r="C105" s="4">
+      <c r="C105" s="3">
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="D105" s="1">
         <v>247831</v>
       </c>
-      <c r="E105" s="4">
+      <c r="E105" s="3">
         <v>0.123</v>
       </c>
       <c r="F105" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>11</v>
       </c>
       <c r="B106" s="1">
         <v>3103</v>
       </c>
-      <c r="C106" s="4">
+      <c r="C106" s="3">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="D106" s="1">
         <v>323609</v>
       </c>
-      <c r="E106" s="4">
+      <c r="E106" s="3">
         <v>0.10199999999999999</v>
       </c>
       <c r="F106" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>12</v>
       </c>
       <c r="B107" s="1">
         <v>443</v>
       </c>
-      <c r="C107" s="4">
+      <c r="C107" s="3">
         <v>0.185</v>
       </c>
       <c r="D107" s="1">
         <v>202969</v>
       </c>
-      <c r="E107" s="4">
+      <c r="E107" s="3">
         <v>0.17299999999999999</v>
       </c>
       <c r="F107" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>13</v>
       </c>
       <c r="B108" s="1">
         <v>4500</v>
       </c>
-      <c r="C108" s="4">
+      <c r="C108" s="3">
         <v>0.23300000000000001</v>
       </c>
       <c r="D108" s="1">
         <v>349780</v>
       </c>
-      <c r="E108" s="4">
+      <c r="E108" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F108" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>14</v>
       </c>
       <c r="B109" s="1">
         <v>518</v>
       </c>
-      <c r="C109" s="4">
+      <c r="C109" s="3">
         <v>0.36699999999999999</v>
       </c>
       <c r="D109" s="1">
         <v>347995</v>
       </c>
-      <c r="E109" s="4">
+      <c r="E109" s="3">
         <v>0.25600000000000001</v>
       </c>
       <c r="F109" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>15</v>
       </c>
       <c r="B110" s="1">
         <v>4197</v>
       </c>
-      <c r="C110" s="4">
+      <c r="C110" s="3">
         <v>0.108</v>
       </c>
       <c r="D110" s="1">
         <v>300514</v>
       </c>
-      <c r="E110" s="4">
+      <c r="E110" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F110" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>16</v>
       </c>
       <c r="B111" s="1">
         <v>4483</v>
       </c>
-      <c r="C111" s="4">
+      <c r="C111" s="3">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="D111" s="1">
         <v>464190</v>
       </c>
-      <c r="E111" s="4">
+      <c r="E111" s="3">
         <v>6.2E-2</v>
       </c>
       <c r="F111" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>17</v>
       </c>
       <c r="B112" s="1">
         <v>333</v>
       </c>
-      <c r="C112" s="4">
+      <c r="C112" s="3">
         <v>0.3</v>
       </c>
       <c r="D112" s="1">
         <v>296260</v>
       </c>
-      <c r="E112" s="4">
+      <c r="E112" s="3">
         <v>0.122</v>
       </c>
       <c r="F112" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>18</v>
       </c>
       <c r="B113" s="1">
         <v>12804</v>
       </c>
-      <c r="C113" s="4">
+      <c r="C113" s="3">
         <v>5.3999999999999999E-2</v>
       </c>
       <c r="D113" s="1">
         <v>554548</v>
       </c>
-      <c r="E113" s="4">
+      <c r="E113" s="3">
         <v>6.3E-2</v>
       </c>
       <c r="F113" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>19</v>
       </c>
       <c r="B114" s="1">
         <v>11610</v>
       </c>
-      <c r="C114" s="4">
+      <c r="C114" s="3">
         <v>-2.8000000000000001E-2</v>
       </c>
       <c r="D114" s="1">
         <v>322660</v>
       </c>
-      <c r="E114" s="4">
+      <c r="E114" s="3">
         <v>0.10299999999999999</v>
       </c>
       <c r="F114" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>20</v>
       </c>
       <c r="B115" s="1">
         <v>875</v>
       </c>
-      <c r="C115" s="4">
+      <c r="C115" s="3">
         <v>0.35799999999999998</v>
       </c>
       <c r="D115" s="1">
         <v>388093</v>
       </c>
-      <c r="E115" s="4">
+      <c r="E115" s="3">
         <v>0.25800000000000001</v>
       </c>
       <c r="F115" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>21</v>
       </c>
       <c r="B116" s="1">
         <v>269</v>
       </c>
-      <c r="C116" s="4">
+      <c r="C116" s="3">
         <v>-0.115</v>
       </c>
       <c r="D116" s="1">
         <v>145486</v>
       </c>
-      <c r="E116" s="4">
+      <c r="E116" s="3">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="F116" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>22</v>
       </c>
       <c r="B117" s="1">
         <v>1850</v>
       </c>
-      <c r="C117" s="4">
+      <c r="C117" s="3">
         <v>0.14199999999999999</v>
       </c>
       <c r="D117" s="1">
         <v>301282</v>
       </c>
-      <c r="E117" s="4">
+      <c r="E117" s="3">
         <v>0.11700000000000001</v>
       </c>
       <c r="F117" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>23</v>
       </c>
       <c r="B118" s="1">
         <v>640</v>
       </c>
-      <c r="C118" s="4">
+      <c r="C118" s="3">
         <v>0.39700000000000002</v>
       </c>
       <c r="D118" s="1">
         <v>518112</v>
       </c>
-      <c r="E118" s="4">
+      <c r="E118" s="3">
         <v>0.23599999999999999</v>
       </c>
       <c r="F118" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>24</v>
       </c>
       <c r="B119" s="1">
         <v>1948</v>
       </c>
-      <c r="C119" s="4">
+      <c r="C119" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="D119" s="1">
         <v>215947</v>
       </c>
-      <c r="E119" s="4">
+      <c r="E119" s="3">
         <v>0.13500000000000001</v>
       </c>
       <c r="F119" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>25</v>
       </c>
       <c r="B120" s="1">
         <v>1213</v>
       </c>
-      <c r="C120" s="4">
+      <c r="C120" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="D120" s="1">
         <v>185596</v>
       </c>
-      <c r="E120" s="4">
+      <c r="E120" s="3">
         <v>0.113</v>
       </c>
       <c r="F120" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>26</v>
       </c>
       <c r="B121" s="1">
         <v>2445</v>
       </c>
-      <c r="C121" s="4">
+      <c r="C121" s="3">
         <v>0.28100000000000003</v>
       </c>
       <c r="D121" s="1">
         <v>295576</v>
       </c>
-      <c r="E121" s="4">
+      <c r="E121" s="3">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="F121" s="1">
         <v>2019</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>3</v>
       </c>
       <c r="B122" s="1">
         <v>769</v>
       </c>
-      <c r="C122" s="4">
+      <c r="C122" s="3">
         <v>0.11600000000000001</v>
       </c>
       <c r="D122" s="1">
         <v>125067</v>
       </c>
-      <c r="E122" s="4">
+      <c r="E122" s="3">
         <v>0.13400000000000001</v>
       </c>
       <c r="F122" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>4</v>
       </c>
       <c r="B123" s="1">
         <v>11316</v>
       </c>
-      <c r="C123" s="4">
+      <c r="C123" s="3">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="D123" s="1">
         <v>450782</v>
       </c>
-      <c r="E123" s="4">
+      <c r="E123" s="3">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="F123" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>5</v>
       </c>
       <c r="B124" s="1">
         <v>9877</v>
       </c>
-      <c r="C124" s="4">
+      <c r="C124" s="3">
         <v>0.187</v>
       </c>
       <c r="D124" s="1">
         <v>206655</v>
       </c>
-      <c r="E124" s="4">
+      <c r="E124" s="3">
         <v>0.161</v>
       </c>
       <c r="F124" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>6</v>
       </c>
       <c r="B125" s="1">
         <v>11713</v>
       </c>
-      <c r="C125" s="4">
+      <c r="C125" s="3">
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="D125" s="1">
         <v>320260</v>
       </c>
-      <c r="E125" s="4">
+      <c r="E125" s="3">
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="F125" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>7</v>
       </c>
       <c r="B126" s="1">
         <v>2027</v>
       </c>
-      <c r="C126" s="4">
+      <c r="C126" s="3">
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="D126" s="1">
         <v>397638</v>
       </c>
-      <c r="E126" s="4">
+      <c r="E126" s="3">
         <v>9.4E-2</v>
       </c>
       <c r="F126" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>8</v>
       </c>
       <c r="B127" s="1">
         <v>444</v>
       </c>
-      <c r="C127" s="4">
+      <c r="C127" s="3">
         <v>0.14599999999999999</v>
       </c>
       <c r="D127" s="1">
         <v>226367</v>
       </c>
-      <c r="E127" s="4">
+      <c r="E127" s="3">
         <v>0.215</v>
       </c>
       <c r="F127" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>9</v>
       </c>
       <c r="B128" s="1">
         <v>2825</v>
       </c>
-      <c r="C128" s="4">
+      <c r="C128" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="D128" s="1">
         <v>380922</v>
       </c>
-      <c r="E128" s="4">
+      <c r="E128" s="3">
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="F128" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>10</v>
       </c>
       <c r="B129" s="1">
         <v>1626</v>
       </c>
-      <c r="C129" s="4">
+      <c r="C129" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D129" s="1">
         <v>278224</v>
       </c>
-      <c r="E129" s="4">
+      <c r="E129" s="3">
         <v>0.10299999999999999</v>
       </c>
       <c r="F129" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>11</v>
       </c>
       <c r="B130" s="1">
         <v>3442</v>
       </c>
-      <c r="C130" s="4">
+      <c r="C130" s="3">
         <v>0.125</v>
       </c>
       <c r="D130" s="1">
         <v>357188</v>
       </c>
-      <c r="E130" s="4">
+      <c r="E130" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="F130" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>12</v>
       </c>
       <c r="B131" s="1">
         <v>527</v>
       </c>
-      <c r="C131" s="4">
+      <c r="C131" s="3">
         <v>0.20100000000000001</v>
       </c>
       <c r="D131" s="1">
         <v>239512</v>
       </c>
-      <c r="E131" s="4">
+      <c r="E131" s="3">
         <v>0.215</v>
       </c>
       <c r="F131" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>13</v>
       </c>
       <c r="B132" s="1">
         <v>5588</v>
       </c>
-      <c r="C132" s="4">
+      <c r="C132" s="3">
         <v>0.104</v>
       </c>
       <c r="D132" s="1">
         <v>382082</v>
       </c>
-      <c r="E132" s="4">
+      <c r="E132" s="3">
         <v>0.153</v>
       </c>
       <c r="F132" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>14</v>
       </c>
       <c r="B133" s="1">
         <v>708</v>
       </c>
-      <c r="C133" s="4">
+      <c r="C133" s="3">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="D133" s="1">
         <v>436946</v>
       </c>
-      <c r="E133" s="4">
+      <c r="E133" s="3">
         <v>0.247</v>
       </c>
       <c r="F133" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>15</v>
       </c>
       <c r="B134" s="1">
         <v>4675</v>
       </c>
-      <c r="C134" s="4">
+      <c r="C134" s="3">
         <v>1.6E-2</v>
       </c>
       <c r="D134" s="1">
         <v>322126</v>
       </c>
-      <c r="E134" s="4">
+      <c r="E134" s="3">
         <v>0.10299999999999999</v>
       </c>
       <c r="F134" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>16</v>
       </c>
       <c r="B135" s="1">
         <v>4723</v>
       </c>
-      <c r="C135" s="4">
+      <c r="C135" s="3">
         <v>0.13</v>
       </c>
       <c r="D135" s="1">
         <v>493944</v>
       </c>
-      <c r="E135" s="4">
+      <c r="E135" s="3">
         <v>0.10100000000000001</v>
       </c>
       <c r="F135" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>17</v>
       </c>
       <c r="B136" s="1">
         <v>433</v>
       </c>
-      <c r="C136" s="4">
+      <c r="C136" s="3">
         <v>0.15</v>
       </c>
       <c r="D136" s="1">
         <v>332523</v>
       </c>
-      <c r="E136" s="4">
+      <c r="E136" s="3">
         <v>0.19900000000000001</v>
       </c>
       <c r="F136" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>18</v>
       </c>
       <c r="B137" s="1">
         <v>13533</v>
       </c>
-      <c r="C137" s="4">
+      <c r="C137" s="3">
         <v>0.158</v>
       </c>
       <c r="D137" s="1">
         <v>589243</v>
       </c>
-      <c r="E137" s="4">
+      <c r="E137" s="3">
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="F137" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>19</v>
       </c>
       <c r="B138" s="1">
         <v>11424</v>
       </c>
-      <c r="C138" s="4">
+      <c r="C138" s="3">
         <v>0.1</v>
       </c>
       <c r="D138" s="1">
         <v>357299</v>
       </c>
-      <c r="E138" s="4">
+      <c r="E138" s="3">
         <v>0.10299999999999999</v>
       </c>
       <c r="F138" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>20</v>
       </c>
       <c r="B139" s="1">
         <v>1192</v>
       </c>
-      <c r="C139" s="4">
+      <c r="C139" s="3">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="D139" s="1">
         <v>488977</v>
       </c>
-      <c r="E139" s="4">
+      <c r="E139" s="3">
         <v>4.7E-2</v>
       </c>
       <c r="F139" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>21</v>
       </c>
       <c r="B140" s="1">
         <v>241</v>
       </c>
-      <c r="C140" s="4">
+      <c r="C140" s="3">
         <v>0.46500000000000002</v>
       </c>
       <c r="D140" s="1">
         <v>159532</v>
       </c>
-      <c r="E140" s="4">
+      <c r="E140" s="3">
         <v>0.20100000000000001</v>
       </c>
       <c r="F140" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>22</v>
       </c>
       <c r="B141" s="1">
         <v>2122</v>
       </c>
-      <c r="C141" s="4">
+      <c r="C141" s="3">
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="D141" s="1">
         <v>336908</v>
       </c>
-      <c r="E141" s="4">
+      <c r="E141" s="3">
         <v>0.10199999999999999</v>
       </c>
       <c r="F141" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>23</v>
       </c>
       <c r="B142" s="1">
         <v>895</v>
       </c>
-      <c r="C142" s="4">
+      <c r="C142" s="3">
         <v>-5.8999999999999997E-2</v>
       </c>
       <c r="D142" s="1">
         <v>640328</v>
       </c>
-      <c r="E142" s="4">
+      <c r="E142" s="3">
         <v>0.129</v>
       </c>
       <c r="F142" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>24</v>
       </c>
       <c r="B143" s="1">
         <v>2070</v>
       </c>
-      <c r="C143" s="4">
+      <c r="C143" s="3">
         <v>0.13900000000000001</v>
       </c>
       <c r="D143" s="1">
         <v>245323</v>
       </c>
-      <c r="E143" s="4">
+      <c r="E143" s="3">
         <v>0.123</v>
       </c>
       <c r="F143" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>25</v>
       </c>
       <c r="B144" s="1">
         <v>1330</v>
       </c>
-      <c r="C144" s="4">
+      <c r="C144" s="3">
         <v>0.17699999999999999</v>
       </c>
       <c r="D144" s="1">
         <v>206589</v>
       </c>
-      <c r="E144" s="4">
+      <c r="E144" s="3">
         <v>0.125</v>
       </c>
       <c r="F144" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>26</v>
       </c>
       <c r="B145" s="1">
         <v>3137</v>
       </c>
-      <c r="C145" s="4">
+      <c r="C145" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
       <c r="D145" s="1">
         <v>323153</v>
       </c>
-      <c r="E145" s="4">
+      <c r="E145" s="3">
         <v>0.23</v>
       </c>
       <c r="F145" s="1">
         <v>2020</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>3</v>
       </c>
       <c r="B146" s="1">
         <v>859</v>
       </c>
-      <c r="C146" s="4">
+      <c r="C146" s="3">
         <v>-8.5999999999999993E-2</v>
       </c>
       <c r="D146" s="1">
         <v>141748</v>
       </c>
-      <c r="E146" s="4">
+      <c r="E146" s="3">
         <v>1.2E-2</v>
       </c>
       <c r="F146" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>4</v>
       </c>
       <c r="B147" s="1">
         <v>12266</v>
       </c>
-      <c r="C147" s="4">
+      <c r="C147" s="3">
         <v>-0.251</v>
       </c>
       <c r="D147" s="1">
         <v>493811</v>
       </c>
-      <c r="E147" s="4">
+      <c r="E147" s="3">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="F147" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>5</v>
       </c>
       <c r="B148" s="1">
         <v>11790</v>
       </c>
-      <c r="C148" s="4">
+      <c r="C148" s="3">
         <v>-0.16400000000000001</v>
       </c>
       <c r="D148" s="1">
         <v>239455</v>
       </c>
-      <c r="E148" s="4">
+      <c r="E148" s="3">
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="F148" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>6</v>
       </c>
       <c r="B149" s="1">
         <v>12905</v>
       </c>
-      <c r="C149" s="4">
+      <c r="C149" s="3">
         <v>-0.19</v>
       </c>
       <c r="D149" s="1">
         <v>350467</v>
       </c>
-      <c r="E149" s="4">
+      <c r="E149" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="F149" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>7</v>
       </c>
       <c r="B150" s="1">
         <v>2192</v>
       </c>
-      <c r="C150" s="4">
+      <c r="C150" s="3">
         <v>-0.3</v>
       </c>
       <c r="D150" s="1">
         <v>434421</v>
       </c>
-      <c r="E150" s="4">
+      <c r="E150" s="3">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="F150" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>8</v>
       </c>
       <c r="B151" s="1">
         <v>510</v>
       </c>
-      <c r="C151" s="4">
+      <c r="C151" s="3">
         <v>-0.182</v>
       </c>
       <c r="D151" s="1">
         <v>275037</v>
       </c>
-      <c r="E151" s="4">
+      <c r="E151" s="3">
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="F151" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>9</v>
       </c>
       <c r="B152" s="1">
         <v>2854</v>
       </c>
-      <c r="C152" s="4">
+      <c r="C152" s="3">
         <v>-0.19</v>
       </c>
       <c r="D152" s="1">
         <v>417441</v>
       </c>
-      <c r="E152" s="4">
+      <c r="E152" s="3">
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="F152" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>10</v>
       </c>
       <c r="B153" s="1">
         <v>1725</v>
       </c>
-      <c r="C153" s="4">
+      <c r="C153" s="3">
         <v>-0.14899999999999999</v>
       </c>
       <c r="D153" s="1">
         <v>307715</v>
       </c>
-      <c r="E153" s="4">
+      <c r="E153" s="3">
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="F153" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>11</v>
       </c>
       <c r="B154" s="1">
         <v>3914</v>
       </c>
-      <c r="C154" s="4">
+      <c r="C154" s="3">
         <v>-0.251</v>
       </c>
       <c r="D154" s="1">
         <v>407570</v>
       </c>
-      <c r="E154" s="4">
+      <c r="E154" s="3">
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="F154" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>12</v>
       </c>
       <c r="B155" s="1">
         <v>633</v>
       </c>
-      <c r="C155" s="4">
+      <c r="C155" s="3">
         <v>-4.2999999999999997E-2</v>
       </c>
       <c r="D155" s="1">
         <v>291058</v>
       </c>
-      <c r="E155" s="4">
+      <c r="E155" s="3">
         <v>0.02</v>
       </c>
       <c r="F155" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>13</v>
       </c>
       <c r="B156" s="1">
         <v>6238</v>
       </c>
-      <c r="C156" s="4">
+      <c r="C156" s="3">
         <v>-0.21</v>
       </c>
       <c r="D156" s="1">
         <v>442527</v>
       </c>
-      <c r="E156" s="4">
+      <c r="E156" s="3">
         <v>0.10299999999999999</v>
       </c>
       <c r="F156" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>14</v>
       </c>
       <c r="B157" s="1">
         <v>734</v>
       </c>
-      <c r="C157" s="4">
+      <c r="C157" s="3">
         <v>-0.27500000000000002</v>
       </c>
       <c r="D157" s="1">
         <v>544657</v>
       </c>
-      <c r="E157" s="4">
+      <c r="E157" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F157" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>15</v>
       </c>
       <c r="B158" s="1">
         <v>4773</v>
       </c>
-      <c r="C158" s="4">
+      <c r="C158" s="3">
         <v>-0.246</v>
       </c>
       <c r="D158" s="1">
         <v>355497</v>
       </c>
-      <c r="E158" s="4">
+      <c r="E158" s="3">
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="F158" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>16</v>
       </c>
       <c r="B159" s="1">
         <v>5367</v>
       </c>
-      <c r="C159" s="4">
+      <c r="C159" s="3">
         <v>-0.21099999999999999</v>
       </c>
       <c r="D159" s="1">
         <v>544662</v>
       </c>
-      <c r="E159" s="4">
+      <c r="E159" s="3">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="F159" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>17</v>
       </c>
       <c r="B160" s="1">
         <v>499</v>
       </c>
-      <c r="C160" s="4">
+      <c r="C160" s="3">
         <v>-0.36499999999999999</v>
       </c>
       <c r="D160" s="1">
         <v>400459</v>
       </c>
-      <c r="E160" s="4">
+      <c r="E160" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F160" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>18</v>
       </c>
       <c r="B161" s="1">
         <v>15718</v>
       </c>
-      <c r="C161" s="4">
+      <c r="C161" s="3">
         <v>-0.23200000000000001</v>
       </c>
       <c r="D161" s="1">
         <v>648172</v>
       </c>
-      <c r="E161" s="4">
+      <c r="E161" s="3">
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="F161" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>19</v>
       </c>
       <c r="B162" s="1">
         <v>12660</v>
       </c>
-      <c r="C162" s="4">
+      <c r="C162" s="3">
         <v>-0.193</v>
       </c>
       <c r="D162" s="1">
         <v>394926</v>
       </c>
-      <c r="E162" s="4">
+      <c r="E162" s="3">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="F162" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>20</v>
       </c>
       <c r="B163" s="1">
         <v>1214</v>
       </c>
-      <c r="C163" s="4">
+      <c r="C163" s="3">
         <v>-0.27800000000000002</v>
       </c>
       <c r="D163" s="1">
         <v>512573</v>
       </c>
-      <c r="E163" s="4">
+      <c r="E163" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="F163" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>21</v>
       </c>
       <c r="B164" s="1">
         <v>354</v>
       </c>
-      <c r="C164" s="4">
+      <c r="C164" s="3">
         <v>-2.8000000000000001E-2</v>
       </c>
       <c r="D164" s="1">
         <v>191526</v>
       </c>
-      <c r="E164" s="4">
+      <c r="E164" s="3">
         <v>0.108</v>
       </c>
       <c r="F164" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>22</v>
       </c>
       <c r="B165" s="1">
         <v>2228</v>
       </c>
-      <c r="C165" s="4">
+      <c r="C165" s="3">
         <v>-0.22</v>
       </c>
       <c r="D165" s="1">
         <v>371612</v>
       </c>
-      <c r="E165" s="4">
+      <c r="E165" s="3">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="F165" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>23</v>
       </c>
       <c r="B166" s="1">
         <v>846</v>
       </c>
-      <c r="C166" s="4">
+      <c r="C166" s="3">
         <v>-0.23599999999999999</v>
       </c>
       <c r="D166" s="1">
         <v>721647</v>
       </c>
-      <c r="E166" s="4">
+      <c r="E166" s="3">
         <v>-3.7999999999999999E-2</v>
       </c>
       <c r="F166" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>24</v>
       </c>
       <c r="B167" s="1">
         <v>2369</v>
       </c>
-      <c r="C167" s="4">
+      <c r="C167" s="3">
         <v>-0.14099999999999999</v>
       </c>
       <c r="D167" s="1">
         <v>275783</v>
       </c>
-      <c r="E167" s="4">
+      <c r="E167" s="3">
         <v>0.10299999999999999</v>
       </c>
       <c r="F167" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>25</v>
       </c>
       <c r="B168" s="1">
         <v>1581</v>
       </c>
-      <c r="C168" s="4">
+      <c r="C168" s="3">
         <v>-0.17399999999999999</v>
       </c>
       <c r="D168" s="1">
         <v>232420</v>
       </c>
-      <c r="E168" s="4">
+      <c r="E168" s="3">
         <v>0.11899999999999999</v>
       </c>
       <c r="F168" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>26</v>
       </c>
       <c r="B169" s="1">
         <v>3178</v>
       </c>
-      <c r="C169" s="4">
+      <c r="C169" s="3">
         <v>-0.28999999999999998</v>
       </c>
       <c r="D169" s="1">
         <v>397774</v>
       </c>
-      <c r="E169" s="4">
+      <c r="E169" s="3">
         <v>0.106</v>
       </c>
       <c r="F169" s="1">
         <v>2021</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>3</v>
       </c>
       <c r="B170" s="1">
         <v>786</v>
       </c>
-      <c r="C170" s="4">
+      <c r="C170" s="3">
         <v>-0.13600000000000001</v>
       </c>
       <c r="D170" s="1">
         <v>143403</v>
       </c>
-      <c r="E170" s="4">
+      <c r="E170" s="3">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="F170" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>4</v>
       </c>
       <c r="B171" s="1">
         <v>9214</v>
       </c>
-      <c r="C171" s="4">
+      <c r="C171" s="3">
         <v>-0.23899999999999999</v>
       </c>
       <c r="D171" s="1">
         <v>531520</v>
       </c>
-      <c r="E171" s="4">
+      <c r="E171" s="3">
         <v>0.06</v>
       </c>
       <c r="F171" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>5</v>
       </c>
       <c r="B172" s="1">
         <v>9905</v>
       </c>
-      <c r="C172" s="4">
+      <c r="C172" s="3">
         <v>-0.17499999999999999</v>
       </c>
       <c r="D172" s="1">
         <v>256875</v>
       </c>
-      <c r="E172" s="4">
+      <c r="E172" s="3">
         <v>-3.2000000000000001E-2</v>
       </c>
       <c r="F172" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>6</v>
       </c>
       <c r="B173" s="1">
         <v>10498</v>
       </c>
-      <c r="C173" s="4">
+      <c r="C173" s="3">
         <v>-0.19400000000000001</v>
       </c>
       <c r="D173" s="1">
         <v>376608</v>
       </c>
-      <c r="E173" s="4">
+      <c r="E173" s="3">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="F173" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>7</v>
       </c>
       <c r="B174" s="1">
         <v>1539</v>
       </c>
-      <c r="C174" s="4">
+      <c r="C174" s="3">
         <v>-0.25700000000000001</v>
       </c>
       <c r="D174" s="1">
         <v>470219</v>
       </c>
-      <c r="E174" s="4">
+      <c r="E174" s="3">
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="F174" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>8</v>
       </c>
       <c r="B175" s="1">
         <v>418</v>
       </c>
-      <c r="C175" s="4">
+      <c r="C175" s="3">
         <v>-0.27500000000000002</v>
       </c>
       <c r="D175" s="1">
         <v>294154</v>
       </c>
-      <c r="E175" s="4">
+      <c r="E175" s="3">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="F175" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>9</v>
       </c>
       <c r="B176" s="1">
         <v>2316</v>
       </c>
-      <c r="C176" s="4">
+      <c r="C176" s="3">
         <v>-0.247</v>
       </c>
       <c r="D176" s="1">
         <v>454604</v>
       </c>
-      <c r="E176" s="4">
+      <c r="E176" s="3">
         <v>5.5E-2</v>
       </c>
       <c r="F176" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>10</v>
       </c>
       <c r="B177" s="1">
         <v>1472</v>
       </c>
-      <c r="C177" s="4">
+      <c r="C177" s="3">
         <v>-0.27300000000000002</v>
       </c>
       <c r="D177" s="1">
         <v>334277</v>
       </c>
-      <c r="E177" s="4">
+      <c r="E177" s="3">
         <v>0.123</v>
       </c>
       <c r="F177" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>11</v>
       </c>
       <c r="B178" s="1">
         <v>2959</v>
       </c>
-      <c r="C178" s="4">
+      <c r="C178" s="3">
         <v>-0.16500000000000001</v>
       </c>
       <c r="D178" s="1">
         <v>442257</v>
       </c>
-      <c r="E178" s="4">
+      <c r="E178" s="3">
         <v>1.9E-2</v>
       </c>
       <c r="F178" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>12</v>
       </c>
       <c r="B179" s="1">
         <v>609</v>
       </c>
-      <c r="C179" s="4">
+      <c r="C179" s="3">
         <v>-0.105</v>
       </c>
       <c r="D179" s="1">
         <v>296597</v>
       </c>
-      <c r="E179" s="4">
+      <c r="E179" s="3">
         <v>2.3E-2</v>
       </c>
       <c r="F179" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>13</v>
       </c>
       <c r="B180" s="1">
         <v>4941</v>
       </c>
-      <c r="C180" s="4">
+      <c r="C180" s="3">
         <v>-0.25600000000000001</v>
       </c>
       <c r="D180" s="1">
         <v>488091</v>
       </c>
-      <c r="E180" s="4">
+      <c r="E180" s="3">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="F180" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>14</v>
       </c>
       <c r="B181" s="1">
         <v>534</v>
       </c>
-      <c r="C181" s="4">
+      <c r="C181" s="3">
         <v>-0.127</v>
       </c>
       <c r="D181" s="1">
         <v>551479</v>
       </c>
-      <c r="E181" s="4">
+      <c r="E181" s="3">
         <v>0.156</v>
       </c>
       <c r="F181" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>15</v>
       </c>
       <c r="B182" s="1">
         <v>3610</v>
       </c>
-      <c r="C182" s="4">
+      <c r="C182" s="3">
         <v>-0.23799999999999999</v>
       </c>
       <c r="D182" s="1">
         <v>380098</v>
       </c>
-      <c r="E182" s="4">
+      <c r="E182" s="3">
         <v>4.7E-2</v>
       </c>
       <c r="F182" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>16</v>
       </c>
       <c r="B183" s="1">
         <v>4237</v>
       </c>
-      <c r="C183" s="4">
+      <c r="C183" s="3">
         <v>-0.20599999999999999</v>
       </c>
       <c r="D183" s="1">
         <v>590526</v>
       </c>
-      <c r="E183" s="4">
+      <c r="E183" s="3">
         <v>5.5E-2</v>
       </c>
       <c r="F183" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>17</v>
       </c>
       <c r="B184" s="1">
         <v>317</v>
       </c>
-      <c r="C184" s="4">
+      <c r="C184" s="3">
         <v>-2.8000000000000001E-2</v>
       </c>
       <c r="D184" s="1">
         <v>410288</v>
       </c>
-      <c r="E184" s="4">
+      <c r="E184" s="3">
         <v>-2.1000000000000001E-2</v>
       </c>
       <c r="F184" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>18</v>
       </c>
       <c r="B185" s="1">
         <v>12102</v>
       </c>
-      <c r="C185" s="4">
+      <c r="C185" s="3">
         <v>-0.23599999999999999</v>
       </c>
       <c r="D185" s="1">
         <v>690155</v>
       </c>
-      <c r="E185" s="4">
+      <c r="E185" s="3">
         <v>0.03</v>
       </c>
       <c r="F185" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>19</v>
       </c>
       <c r="B186" s="1">
         <v>10291</v>
       </c>
-      <c r="C186" s="4">
+      <c r="C186" s="3">
         <v>-0.17299999999999999</v>
       </c>
       <c r="D186" s="1">
         <v>421316</v>
       </c>
-      <c r="E186" s="4">
+      <c r="E186" s="3">
         <v>3.1E-2</v>
       </c>
       <c r="F186" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>20</v>
       </c>
       <c r="B187" s="1">
         <v>879</v>
       </c>
-      <c r="C187" s="4">
+      <c r="C187" s="3">
         <v>-8.2000000000000003E-2</v>
       </c>
       <c r="D187" s="1">
         <v>550807</v>
       </c>
-      <c r="E187" s="4">
+      <c r="E187" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="F187" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>21</v>
       </c>
       <c r="B188" s="1">
         <v>344</v>
       </c>
-      <c r="C188" s="4">
+      <c r="C188" s="3">
         <v>-0.23799999999999999</v>
       </c>
       <c r="D188" s="1">
         <v>212199</v>
       </c>
-      <c r="E188" s="4">
+      <c r="E188" s="3">
         <v>-7.2999999999999995E-2</v>
       </c>
       <c r="F188" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>22</v>
       </c>
       <c r="B189" s="1">
         <v>1740</v>
       </c>
-      <c r="C189" s="4">
+      <c r="C189" s="3">
         <v>-0.20399999999999999</v>
       </c>
       <c r="D189" s="1">
         <v>399530</v>
       </c>
-      <c r="E189" s="4">
+      <c r="E189" s="3">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="F189" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>23</v>
       </c>
       <c r="B190" s="1">
         <v>646</v>
       </c>
-      <c r="C190" s="4">
+      <c r="C190" s="3">
         <v>-0.218</v>
       </c>
       <c r="D190" s="1">
         <v>693912</v>
       </c>
-      <c r="E190" s="4">
+      <c r="E190" s="3">
         <v>0.13900000000000001</v>
       </c>
       <c r="F190" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>24</v>
       </c>
       <c r="B191" s="1">
         <v>2043</v>
       </c>
-      <c r="C191" s="4">
+      <c r="C191" s="3">
         <v>-0.17</v>
       </c>
       <c r="D191" s="1">
         <v>304290</v>
       </c>
-      <c r="E191" s="4">
+      <c r="E191" s="3">
         <v>6.0999999999999999E-2</v>
       </c>
       <c r="F191" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>25</v>
       </c>
       <c r="B192" s="1">
         <v>1309</v>
       </c>
-      <c r="C192" s="4">
+      <c r="C192" s="3">
         <v>-0.191</v>
       </c>
       <c r="D192" s="1">
         <v>260007</v>
       </c>
-      <c r="E192" s="4">
+      <c r="E192" s="3">
         <v>3.9E-2</v>
       </c>
       <c r="F192" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>26</v>
       </c>
       <c r="B193" s="1">
         <v>2258</v>
       </c>
-      <c r="C193" s="4">
+      <c r="C193" s="3">
         <v>-0.14799999999999999</v>
       </c>
       <c r="D193" s="1">
         <v>439993</v>
       </c>
-      <c r="E193" s="4">
+      <c r="E193" s="3">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="F193" s="1">
         <v>2022</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>3</v>
       </c>
@@ -4389,7 +4395,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>4</v>
       </c>
@@ -4403,7 +4409,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>5</v>
       </c>
@@ -4417,7 +4423,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>6</v>
       </c>
@@ -4431,7 +4437,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>7</v>
       </c>
@@ -4445,7 +4451,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>8</v>
       </c>
@@ -4459,7 +4465,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>9</v>
       </c>
@@ -4473,7 +4479,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>10</v>
       </c>
@@ -4487,7 +4493,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>11</v>
       </c>
@@ -4501,7 +4507,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>12</v>
       </c>
@@ -4515,7 +4521,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>13</v>
       </c>
@@ -4529,7 +4535,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>14</v>
       </c>
@@ -4543,7 +4549,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>15</v>
       </c>
@@ -4557,7 +4563,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>16</v>
       </c>
@@ -4571,7 +4577,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>17</v>
       </c>
@@ -4585,7 +4591,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>18</v>
       </c>
@@ -4599,7 +4605,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>19</v>
       </c>
@@ -4613,7 +4619,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>20</v>
       </c>
@@ -4627,7 +4633,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>21</v>
       </c>
@@ -4641,7 +4647,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>22</v>
       </c>
@@ -4655,7 +4661,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>23</v>
       </c>
@@ -4669,7 +4675,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>24</v>
       </c>
@@ -4683,7 +4689,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>25</v>
       </c>
@@ -4697,7 +4703,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>26</v>
       </c>

</xml_diff>